<commit_message>
Revised default_admin.xlsx to include previous calibration info
and whether the weights are new, and a notes section in case it's handy
</commit_message>
<xml_diff>
--- a/mass_circular_weighing/utils/default_admin.xlsx
+++ b/mass_circular_weighing/utils/default_admin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\mass_circular_weighing\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca.hawke\PycharmProjects\Mass-Circular-Weighing\mass_circular_weighing\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4E47B2-E331-4880-A11A-AB78FD6AF677}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3706983-8B2B-467D-93E4-826CA2551476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24885" yWindow="3375" windowWidth="18810" windowHeight="10275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32025" yWindow="2100" windowWidth="21240" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>Title</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Path to xlsx of standard masses</t>
   </si>
   <si>
-    <t>G:\Shared drives\MSL - MAP\mass_setfiles\MASSREF19_4MCW.xlsx</t>
-  </si>
-  <si>
     <t>Mettler A</t>
   </si>
   <si>
@@ -229,7 +226,22 @@
     <t>default</t>
   </si>
   <si>
-    <t>G:\My Drive</t>
+    <t>New weights?</t>
+  </si>
+  <si>
+    <t>&lt; add any additional notes over here &gt;</t>
+  </si>
+  <si>
+    <t>I:\MSL\Private\Mass\Commercial Calibrations</t>
+  </si>
+  <si>
+    <t>Previous Calibration</t>
+  </si>
+  <si>
+    <t>I:\MSL\Private\Mass\MassSets\MASSREF19_4MCW.xlsx</t>
+  </si>
+  <si>
+    <t>C:\MCW_Config\local_config.xml</t>
   </si>
 </sst>
 </file>
@@ -311,12 +323,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -324,17 +333,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -353,13 +356,32 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -703,236 +725,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="41.81640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="16" style="21" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="21" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="2" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="I2" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+    </row>
+    <row r="3" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="F5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="34"/>
+      <c r="G11" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="14"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" s="17"/>
-      <c r="D12" s="16"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="H14" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="11">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>100</v>
       </c>
       <c r="B15" s="1">
         <v>100</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -942,14 +1002,14 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="1">
         <v>200</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -959,14 +1019,14 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="1">
         <v>200</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -976,367 +1036,371 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="18"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="18"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="18"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="18"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="18"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="18"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="11"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="18"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="18"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="11"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="18"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="18"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="11"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="18"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="18"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="11"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="18"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="11"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="18"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="11"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="18"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="18"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="18"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="18"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="11"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="18"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="18"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="11"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="18"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="11"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="18"/>
+      <c r="C39" s="17"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="11"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="18"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="11"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="18"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="11"/>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="18"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="11"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="18"/>
+      <c r="C43" s="17"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="11"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="18"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="11"/>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="18"/>
+      <c r="C45" s="17"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="11"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="18"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="11"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="18"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="11"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="18"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="11"/>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="18"/>
+      <c r="C49" s="17"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="11"/>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="18"/>
+      <c r="C50" s="17"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="11"/>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="18"/>
+      <c r="C51" s="17"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="11"/>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="18"/>
+      <c r="C52" s="17"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="11"/>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="18"/>
+      <c r="C53" s="17"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="11"/>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="18"/>
+      <c r="C54" s="17"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="11"/>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="18"/>
+      <c r="C55" s="17"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B1:C1"/>
+  <mergeCells count="11">
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{8A755FC5-F8A9-4556-81DF-DEAB3CAEEEBC}">
       <formula1>"auto select, linear drift, quadratic drift, cubic drift"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{FA295EA3-D276-4F59-867E-430B0245CCAF}">
       <formula1>"NO, YES"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{8ACFD20D-2222-4384-B93F-40FD733FA330}">
+      <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1350,29 +1414,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="24.36328125" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
tests for TP009 and IRL955
Tests for buoyancy corrections, and uncertainty contributions from air density, volumes, and heights of COMs.

Structure of admin file has changed to include COM heights and uncertainties
</commit_message>
<xml_diff>
--- a/mass_circular_weighing/utils/default_admin.xlsx
+++ b/mass_circular_weighing/utils/default_admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca.hawke\PycharmProjects\Mass-Circular-Weighing\mass_circular_weighing\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\mass_circular_weighing\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3706983-8B2B-467D-93E4-826CA2551476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A238A68-8FB8-44C7-B8F8-AA0A8740DC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="2100" windowWidth="21240" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Title</t>
   </si>
@@ -70,12 +70,6 @@
     <t>The J-number job code for the calibration</t>
   </si>
   <si>
-    <t>Project Number</t>
-  </si>
-  <si>
-    <t>96240….</t>
-  </si>
-  <si>
     <t>Save folder</t>
   </si>
   <si>
@@ -85,18 +79,12 @@
     <t>Report Number</t>
   </si>
   <si>
-    <t>Mass/2021/0000</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Drift correction</t>
   </si>
   <si>
-    <t>auto select</t>
-  </si>
-  <si>
     <t>Specify a drift option to use in the least squares analysis of each circular weighing. Allowed options: auto select, linear drift, quadratic drift, cubic drift</t>
   </si>
   <si>
@@ -115,9 +103,6 @@
     <t>Correlations</t>
   </si>
   <si>
-    <t>If relevant, include a matrix/list of correlations between standards (e.g. in build-up or build-down). Allowed options: None, or matrix of correlations</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -241,14 +226,45 @@
     <t>I:\MSL\Private\Mass\MassSets\MASSREF19_4MCW.xlsx</t>
   </si>
   <si>
-    <t>C:\MCW_Config\local_config.xml</t>
+    <t>Expansion coeff (ppm/degC)</t>
+  </si>
+  <si>
+    <t>Number of weights</t>
+  </si>
+  <si>
+    <t>(calculated automatically)</t>
+  </si>
+  <si>
+    <t>linear drift</t>
+  </si>
+  <si>
+    <t>Correct for air density?</t>
+  </si>
+  <si>
+    <t>If true, calculate basis 8000 mass differences using measured air density. Requires densities and expansion coefficients for all masses.</t>
+  </si>
+  <si>
+    <t>tests\samples\config_fmc.xml</t>
+  </si>
+  <si>
+    <t>If relevant, include a matrix of correlations between standards (e.g. in build-up or build-down). Allowed options: None, or 2x2 matrix of correlations</t>
+  </si>
+  <si>
+    <t>Mass/YEAR/0000</t>
+  </si>
+  <si>
+    <t>JIRA Project Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +306,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -320,8 +346,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -373,7 +400,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -381,6 +407,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -407,13 +442,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{8687DA4F-417B-4933-B759-FA9A7445193C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -429,9 +461,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -469,7 +501,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -575,7 +607,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -717,7 +749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -728,69 +760,68 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="16" style="21" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="21"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G2" s="7"/>
-      <c r="I2" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
+      <c r="I2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
     </row>
     <row r="3" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -798,15 +829,15 @@
       <c r="D3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
@@ -819,130 +850,150 @@
         <v>11</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
+        <v>73</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>67</v>
+        <v>72</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-    </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+    </row>
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="7" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="26"/>
+        <v>15</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="26"/>
+        <v>18</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="16"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -951,38 +1002,50 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="29"/>
-      <c r="F13" s="11"/>
+        <v>27</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="31"/>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13">
+        <f>COUNT(B15:B90)</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="G14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -993,50 +1056,53 @@
         <v>100</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1">
         <v>200</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1">
         <v>200</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="1"/>
       <c r="C18" s="17"/>
@@ -1044,8 +1110,9 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="17"/>
@@ -1053,8 +1120,9 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="1"/>
       <c r="C20" s="17"/>
@@ -1062,8 +1130,9 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="1"/>
       <c r="C21" s="17"/>
@@ -1071,8 +1140,9 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="1"/>
       <c r="C22" s="17"/>
@@ -1080,8 +1150,9 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="1"/>
       <c r="C23" s="17"/>
@@ -1089,8 +1160,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="1"/>
       <c r="C24" s="17"/>
@@ -1098,8 +1170,9 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="1"/>
       <c r="C25" s="17"/>
@@ -1107,8 +1180,9 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="17"/>
@@ -1116,8 +1190,9 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="1"/>
       <c r="C27" s="17"/>
@@ -1125,8 +1200,9 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="1"/>
       <c r="C28" s="17"/>
@@ -1134,8 +1210,9 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="1"/>
       <c r="C29" s="17"/>
@@ -1143,8 +1220,9 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="1"/>
       <c r="C30" s="17"/>
@@ -1152,8 +1230,9 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="1"/>
       <c r="C31" s="17"/>
@@ -1161,8 +1240,9 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="1"/>
       <c r="C32" s="17"/>
@@ -1170,8 +1250,9 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="1"/>
       <c r="C33" s="17"/>
@@ -1179,8 +1260,9 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="17"/>
@@ -1188,8 +1270,9 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="17"/>
@@ -1197,8 +1280,9 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="1"/>
       <c r="C36" s="17"/>
@@ -1206,8 +1290,9 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="1"/>
       <c r="C37" s="17"/>
@@ -1215,8 +1300,9 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="1"/>
       <c r="C38" s="17"/>
@@ -1224,8 +1310,9 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="1"/>
       <c r="C39" s="17"/>
@@ -1233,8 +1320,9 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="1"/>
       <c r="C40" s="17"/>
@@ -1242,8 +1330,9 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="1"/>
       <c r="C41" s="17"/>
@@ -1251,8 +1340,9 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="1"/>
       <c r="C42" s="17"/>
@@ -1260,8 +1350,9 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="1"/>
       <c r="C43" s="17"/>
@@ -1269,8 +1360,9 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="1"/>
       <c r="C44" s="17"/>
@@ -1278,8 +1370,9 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="1"/>
       <c r="C45" s="17"/>
@@ -1287,8 +1380,9 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="1"/>
       <c r="C46" s="17"/>
@@ -1296,8 +1390,9 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="1"/>
       <c r="C47" s="17"/>
@@ -1305,8 +1400,9 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="17"/>
@@ -1314,8 +1410,9 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="1"/>
       <c r="C49" s="17"/>
@@ -1323,8 +1420,9 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="1"/>
       <c r="C50" s="17"/>
@@ -1332,8 +1430,9 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="1"/>
       <c r="C51" s="17"/>
@@ -1341,8 +1440,9 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="1"/>
       <c r="C52" s="17"/>
@@ -1350,8 +1450,9 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="1"/>
       <c r="C53" s="17"/>
@@ -1359,8 +1460,9 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="17"/>
@@ -1368,8 +1470,9 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="1"/>
       <c r="C55" s="17"/>
@@ -1377,6 +1480,7 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1384,19 +1488,19 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
-    <mergeCell ref="E11:F11"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I7:N7"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{8A755FC5-F8A9-4556-81DF-DEAB3CAEEEBC}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{D796BA49-4728-43E1-B665-4473B7CE380D}">
       <formula1>"auto select, linear drift, quadratic drift, cubic drift"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{FA295EA3-D276-4F59-867E-430B0245CCAF}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{B09FC796-A6A9-4E0F-814E-06E996F2419A}">
       <formula1>"NO, YES"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{8ACFD20D-2222-4384-B93F-40FD733FA330}">
@@ -1424,30 +1528,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
helper script for fmc_popup
to run the circular weighing program for analysis without the gui
</commit_message>
<xml_diff>
--- a/mass_circular_weighing/utils/default_admin.xlsx
+++ b/mass_circular_weighing/utils/default_admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\mass_circular_weighing\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A238A68-8FB8-44C7-B8F8-AA0A8740DC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8123FC98-E1C1-4C4D-B9CE-7A954C5DF43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29415" yWindow="1605" windowWidth="26115" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
   <si>
     <t>Title</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Client full address</t>
   </si>
   <si>
-    <t>Job Number</t>
-  </si>
-  <si>
     <t>J00000</t>
   </si>
   <si>
@@ -254,6 +251,15 @@
   </si>
   <si>
     <t>JIRA Project Number</t>
+  </si>
+  <si>
+    <t>Centre Height (mm)</t>
+  </si>
+  <si>
+    <t>u_height (mm)</t>
+  </si>
+  <si>
+    <t>Project Number</t>
   </si>
 </sst>
 </file>
@@ -415,32 +421,32 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -760,7 +766,7 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,49 +785,49 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="I2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="I2" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -829,9 +835,9 @@
       <c r="D3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -841,16 +847,16 @@
     </row>
     <row r="4" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="6"/>
       <c r="I4" s="22"/>
@@ -862,22 +868,22 @@
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="D5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>62</v>
       </c>
       <c r="G5" s="7"/>
       <c r="I5" s="22"/>
@@ -889,52 +895,52 @@
     </row>
     <row r="6" spans="1:14" s="16" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
     </row>
     <row r="8" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="F8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="L8" s="25"/>
@@ -942,25 +948,25 @@
     </row>
     <row r="9" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="F9" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="L9" s="25"/>
@@ -968,32 +974,32 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1002,50 +1008,56 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="27"/>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13">
         <f>COUNT(B15:B90)</f>
         <v>3</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" t="s">
-        <v>35</v>
+        <v>63</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1056,53 +1068,59 @@
         <v>100</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>200</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1">
         <v>200</v>
       </c>
       <c r="C17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="1"/>
       <c r="C18" s="17"/>
@@ -1111,8 +1129,10 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="17"/>
@@ -1121,8 +1141,10 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="1"/>
       <c r="C20" s="17"/>
@@ -1131,8 +1153,10 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="1"/>
       <c r="C21" s="17"/>
@@ -1141,8 +1165,10 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="1"/>
       <c r="C22" s="17"/>
@@ -1151,8 +1177,10 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="1"/>
       <c r="C23" s="17"/>
@@ -1161,8 +1189,10 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="1"/>
       <c r="C24" s="17"/>
@@ -1171,8 +1201,10 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="1"/>
       <c r="C25" s="17"/>
@@ -1181,8 +1213,10 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="17"/>
@@ -1191,8 +1225,10 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="1"/>
       <c r="C27" s="17"/>
@@ -1201,8 +1237,10 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="1"/>
       <c r="C28" s="17"/>
@@ -1211,8 +1249,10 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="1"/>
       <c r="C29" s="17"/>
@@ -1221,8 +1261,10 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="1"/>
       <c r="C30" s="17"/>
@@ -1231,8 +1273,10 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="1"/>
       <c r="C31" s="17"/>
@@ -1241,8 +1285,10 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="1"/>
       <c r="C32" s="17"/>
@@ -1251,8 +1297,10 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="1"/>
       <c r="C33" s="17"/>
@@ -1261,8 +1309,10 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="17"/>
@@ -1271,8 +1321,10 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="17"/>
@@ -1281,8 +1333,10 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="1"/>
       <c r="C36" s="17"/>
@@ -1291,8 +1345,10 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="1"/>
       <c r="C37" s="17"/>
@@ -1301,8 +1357,10 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="1"/>
       <c r="C38" s="17"/>
@@ -1311,8 +1369,10 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="1"/>
       <c r="C39" s="17"/>
@@ -1321,8 +1381,10 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="1"/>
       <c r="C40" s="17"/>
@@ -1331,8 +1393,10 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="1"/>
       <c r="C41" s="17"/>
@@ -1341,8 +1405,10 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="1"/>
       <c r="C42" s="17"/>
@@ -1351,8 +1417,10 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="1"/>
       <c r="C43" s="17"/>
@@ -1361,8 +1429,10 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="1"/>
       <c r="C44" s="17"/>
@@ -1371,8 +1441,10 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="1"/>
       <c r="C45" s="17"/>
@@ -1381,8 +1453,10 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="1"/>
       <c r="C46" s="17"/>
@@ -1391,8 +1465,10 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="1"/>
       <c r="C47" s="17"/>
@@ -1401,8 +1477,10 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="17"/>
@@ -1411,8 +1489,10 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="1"/>
       <c r="C49" s="17"/>
@@ -1421,8 +1501,10 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="1"/>
       <c r="C50" s="17"/>
@@ -1431,8 +1513,10 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="1"/>
       <c r="C51" s="17"/>
@@ -1441,8 +1525,10 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="1"/>
       <c r="C52" s="17"/>
@@ -1451,8 +1537,10 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="1"/>
       <c r="C53" s="17"/>
@@ -1461,8 +1549,10 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="17"/>
@@ -1471,8 +1561,10 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="1"/>
       <c r="C55" s="17"/>
@@ -1481,9 +1573,14 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I7:N7"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="F7:H7"/>
@@ -1492,9 +1589,6 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I7:N7"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{D796BA49-4728-43E1-B665-4473B7CE380D}">
@@ -1528,30 +1622,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
default admin for v2
suitable for scale realisation
</commit_message>
<xml_diff>
--- a/mass_circular_weighing/utils/default_admin.xlsx
+++ b/mass_circular_weighing/utils/default_admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\mass_circular_weighing\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8123FC98-E1C1-4C4D-B9CE-7A954C5DF43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD609DD-1BD3-475B-A27B-691E525CF790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29415" yWindow="1605" windowWidth="26115" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -241,9 +241,6 @@
     <t>If true, calculate basis 8000 mass differences using measured air density. Requires densities and expansion coefficients for all masses.</t>
   </si>
   <si>
-    <t>tests\samples\config_fmc.xml</t>
-  </si>
-  <si>
     <t>If relevant, include a matrix of correlations between standards (e.g. in build-up or build-down). Allowed options: None, or 2x2 matrix of correlations</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>Project Number</t>
+  </si>
+  <si>
+    <t>C:\MCW_Config\local_config.xml</t>
   </si>
 </sst>
 </file>
@@ -421,21 +421,24 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -444,9 +447,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -766,7 +766,7 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,18 +785,18 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -813,14 +813,14 @@
         <v>58</v>
       </c>
       <c r="G2" s="7"/>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
     </row>
     <row r="3" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -835,9 +835,9 @@
       <c r="D3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -847,7 +847,7 @@
     </row>
     <row r="4" spans="1:14" s="20" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>9</v>
@@ -856,7 +856,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="6"/>
       <c r="I4" s="22"/>
@@ -880,7 +880,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>61</v>
@@ -902,45 +902,45 @@
       <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
     </row>
     <row r="8" spans="1:14" s="16" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="L8" s="25"/>
@@ -962,11 +962,11 @@
       <c r="E9" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="L9" s="25"/>
@@ -995,7 +995,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="11" t="s">
@@ -1010,7 +1010,7 @@
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="27"/>
@@ -1054,10 +1054,10 @@
         <v>63</v>
       </c>
       <c r="I14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>